<commit_message>
Improved testing methods for REG Scenario
</commit_message>
<xml_diff>
--- a/Data Files/Web/REG_Birthday.xlsx
+++ b/Data Files/Web/REG_Birthday.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rizki\git\CodingID-QA\Data Files\Web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D753D0-8D50-48B3-91C8-7FA3DC31F043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87962E0-6D61-4C74-AB1B-1A43C949767B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{16B306DF-9094-4C0A-A032-600CADA8B366}"/>
+    <workbookView xWindow="2820" yWindow="1575" windowWidth="21600" windowHeight="11295" xr2:uid="{16B306DF-9094-4C0A-A032-600CADA8B366}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -406,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7750AEF7-008C-4E86-A139-391D3CF712DA}">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A7" sqref="A7:A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,36 +447,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>